<commit_message>
Script pour exporter notes étudiants
</commit_message>
<xml_diff>
--- a/tp1-template.xlsx
+++ b/tp1-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\MAVERICK\Users\Sebastien\ETS\5_E2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sebastien\Documents\ETS\mes-scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E765DE82-EDC2-44E1-B254-FDDD0CA37DA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5DEF59-FE22-4DA9-8421-4559F61D877B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -578,7 +578,7 @@
   <dimension ref="A1:E1024"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>